<commit_message>
Redid some of the examples
</commit_message>
<xml_diff>
--- a/misc/housing/housing_different_levels_results.xlsx
+++ b/misc/housing/housing_different_levels_results.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG14"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,40 +566,35 @@
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>univariate</t>
+          <t>models</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>models</t>
+          <t>weights</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>weights</t>
+          <t>LevelTestSetRMSE</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>LevelTestSetRMSE</t>
+          <t>LevelTestSetMAPE</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>LevelTestSetMAPE</t>
+          <t>LevelTestSetMAE</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>LevelTestSetMAE</t>
+          <t>LevelTestSetR2</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>LevelTestSetR2</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>best_model</t>
         </is>
@@ -608,28 +603,38 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>weighted_diff</t>
+          <t>knn</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>combo</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>knn</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>['AR1', 'AR2', 'AR3', 'AR4', 'AR12', 'AR24', 'monthsin', 'monthcos', 'year', 'COVID19', 't', 't_COVID19']</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'how': 'weighted', 'models': ('knn', 'svr', 'lightgbm', 'mlp', 'elasticnet'), 'determine_best_by': 'ValidationMetricValue'}</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>{'n_neighbors': 9, 'weights': 'uniform'}</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>minmax</t>
+        </is>
+      </c>
       <c r="F2" t="n">
         <v>749</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
       <c r="I2" t="n">
         <v>1</v>
       </c>
@@ -637,19 +642,19 @@
         <v>12</v>
       </c>
       <c r="K2" t="n">
-        <v>13.69987632877164</v>
+        <v>12.90048727825662</v>
       </c>
       <c r="L2" t="n">
-        <v>4.332914524672197</v>
+        <v>3.410422048865689</v>
       </c>
       <c r="M2" t="n">
-        <v>10.27700885310714</v>
+        <v>10.2037037037037</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1457818756160046</v>
+        <v>0.2425609038133143</v>
       </c>
       <c r="O2" t="n">
-        <v>8.372479758335343</v>
+        <v>0.2111111111111094</v>
       </c>
       <c r="P2" t="n">
         <v>8.600000000000023</v>
@@ -658,45 +663,44 @@
         <v>0.95</v>
       </c>
       <c r="R2" t="n">
-        <v>23.20596332465039</v>
+        <v>16.41216392929453</v>
       </c>
       <c r="S2" t="n">
-        <v>11.40415825016577</v>
+        <v>9.843431419125272</v>
       </c>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="n">
-        <v>8.859377765531843</v>
+        <v>7.66327969348659</v>
       </c>
       <c r="V2" t="n">
-        <v>0.5489086944779842</v>
-      </c>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
+        <v>0.6639290096719305</v>
+      </c>
+      <c r="W2" t="n">
+        <v>6</v>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="Y2" t="n">
+        <v>17.29423117975371</v>
+      </c>
       <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>['elasticnet', 'mlp', 'svr', 'knn', 'lightgbm']</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>(0.3507344282636684, 0.30000338225483425, 0.22729266893575065, 0.0900845725217768, 0.03188494802396986)</t>
-        </is>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="n">
+        <v>10.68541899095892</v>
       </c>
       <c r="AC2" t="n">
-        <v>10.93267311340911</v>
+        <v>0.06513677577224607</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.07037192623920496</v>
+        <v>8.617592592592581</v>
       </c>
       <c r="AE2" t="n">
-        <v>9.220536865235905</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0.4207760663045943</v>
-      </c>
-      <c r="AG2" t="b">
+        <v>0.4466793413530572</v>
+      </c>
+      <c r="AF2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -718,10 +722,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{'alpha': 1.3, 'l1_ratio': 1.0}</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>{'alpha': 2.0, 'l1_ratio': 0.0}</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>minmax</t>
+        </is>
+      </c>
       <c r="F3" t="n">
         <v>749</v>
       </c>
@@ -738,19 +746,19 @@
         <v>12</v>
       </c>
       <c r="K3" t="n">
-        <v>14.02642592524194</v>
+        <v>14.88100405815091</v>
       </c>
       <c r="L3" t="n">
-        <v>6.663780491287947</v>
+        <v>0.9551364952389999</v>
       </c>
       <c r="M3" t="n">
-        <v>10.2331159818476</v>
+        <v>11.28436423496344</v>
       </c>
       <c r="N3" t="n">
-        <v>0.104574344698823</v>
+        <v>-0.00785941843021809</v>
       </c>
       <c r="O3" t="n">
-        <v>8.795879531155014</v>
+        <v>0.5765355986389751</v>
       </c>
       <c r="P3" t="n">
         <v>8.600000000000023</v>
@@ -759,17 +767,17 @@
         <v>0.95</v>
       </c>
       <c r="R3" t="n">
-        <v>19.89415650502244</v>
+        <v>36.26046623382577</v>
       </c>
       <c r="S3" t="n">
-        <v>12.05240000938119</v>
+        <v>16.57315668656007</v>
       </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
-        <v>9.386526075224372</v>
+        <v>12.34045324415491</v>
       </c>
       <c r="V3" t="n">
-        <v>0.4961687971781187</v>
+        <v>0.04731690545640299</v>
       </c>
       <c r="W3" t="n">
         <v>6</v>
@@ -780,31 +788,30 @@
         </is>
       </c>
       <c r="Y3" t="n">
-        <v>9.710460564204618</v>
+        <v>13.80960131137844</v>
       </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
+      <c r="AB3" t="n">
+        <v>17.33300005326848</v>
+      </c>
       <c r="AC3" t="n">
-        <v>12.83287437311246</v>
+        <v>0.1011041181960743</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.08414943396922821</v>
+        <v>13.74240056805286</v>
       </c>
       <c r="AE3" t="n">
-        <v>11.11989880828007</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>0.2019287636698676</v>
-      </c>
-      <c r="AG3" t="b">
+        <v>-0.4559325300193688</v>
+      </c>
+      <c r="AF3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>avg_diff</t>
+          <t>weighted_diff</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -815,7 +822,7 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{'how': 'simple', 'models': ('knn', 'svr', 'lightgbm', 'mlp', 'elasticnet'), 'determine_best_by': 'ValidationMetricValue'}</t>
+          <t>{'how': 'weighted', 'models': ('knn', 'svr', 'lightgbm', 'mlp', 'elasticnet'), 'determine_best_by': 'ValidationMetricValue'}</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -833,19 +840,19 @@
         <v>12</v>
       </c>
       <c r="K4" t="n">
-        <v>13.82569459573342</v>
+        <v>13.66953116542876</v>
       </c>
       <c r="L4" t="n">
-        <v>3.218737465945921</v>
+        <v>2.195778392132696</v>
       </c>
       <c r="M4" t="n">
-        <v>10.56365533622696</v>
+        <v>10.73984302671501</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1300197231909647</v>
+        <v>0.1495618631159008</v>
       </c>
       <c r="O4" t="n">
-        <v>5.8779974113453</v>
+        <v>3.304826899731122</v>
       </c>
       <c r="P4" t="n">
         <v>8.600000000000023</v>
@@ -854,79 +861,72 @@
         <v>0.95</v>
       </c>
       <c r="R4" t="n">
-        <v>23.23975459427106</v>
+        <v>23.04758079529754</v>
       </c>
       <c r="S4" t="n">
-        <v>10.6878676822352</v>
+        <v>12.85268264124906</v>
       </c>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="n">
-        <v>8.328465558731358</v>
+        <v>9.781720693145012</v>
       </c>
       <c r="V4" t="n">
-        <v>0.6037948438064218</v>
+        <v>0.4270383501647865</v>
       </c>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>['elasticnet', 'mlp', 'svr', 'knn', 'lightgbm']</t>
+        </is>
+      </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>['knn', 'svr', 'lightgbm', 'mlp', 'elasticnet']</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr"/>
+          <t>(0.34887849314711705, 0.24452653501067947, 0.21811370061682236, 0.1567650445756432, 0.03171622664973791)</t>
+        </is>
+      </c>
+      <c r="AB4" t="n">
+        <v>16.92681824432916</v>
+      </c>
       <c r="AC4" t="n">
-        <v>13.62333173146404</v>
+        <v>0.1114415234512307</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.08906940354174113</v>
+        <v>14.93000405785088</v>
       </c>
       <c r="AE4" t="n">
-        <v>11.86658207438018</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>0.1005843569058439</v>
-      </c>
-      <c r="AG4" t="b">
+        <v>-0.3884953661113768</v>
+      </c>
+      <c r="AF4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>knn</t>
+          <t>avg_diff</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>knn</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>['AR1', 'AR2', 'AR3', 'AR4', 'AR12', 'AR24', 'monthsin', 'monthcos', 'year', 'COVID19', 't', 't_COVID19']</t>
-        </is>
-      </c>
+          <t>combo</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>{'n_neighbors': 20, 'weights': 'uniform'}</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>minmax</t>
-        </is>
-      </c>
+          <t>{'how': 'simple', 'models': ('knn', 'svr', 'lightgbm', 'mlp', 'elasticnet'), 'determine_best_by': 'ValidationMetricValue'}</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
         <v>749</v>
       </c>
       <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>1</v>
       </c>
@@ -934,19 +934,19 @@
         <v>12</v>
       </c>
       <c r="K5" t="n">
-        <v>13.84369388626701</v>
+        <v>13.70574451313872</v>
       </c>
       <c r="L5" t="n">
-        <v>0.9462597100450439</v>
+        <v>2.334770428481689</v>
       </c>
       <c r="M5" t="n">
-        <v>10.74541666666666</v>
+        <v>10.89777822795226</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1277530420227245</v>
+        <v>0.1450499298828504</v>
       </c>
       <c r="O5" t="n">
-        <v>2.39</v>
+        <v>2.60513093622643</v>
       </c>
       <c r="P5" t="n">
         <v>8.600000000000023</v>
@@ -955,57 +955,52 @@
         <v>0.95</v>
       </c>
       <c r="R5" t="n">
-        <v>16.4882467956581</v>
+        <v>24.86799205672756</v>
       </c>
       <c r="S5" t="n">
-        <v>10.41035788413934</v>
+        <v>11.44420562404175</v>
       </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="n">
-        <v>8.125675862068965</v>
+        <v>8.812494076431962</v>
       </c>
       <c r="V5" t="n">
-        <v>0.6241026139300599</v>
-      </c>
-      <c r="W5" t="n">
-        <v>6</v>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>rmse</t>
-        </is>
-      </c>
-      <c r="Y5" t="n">
-        <v>16.34484041932907</v>
-      </c>
-      <c r="Z5" t="inlineStr"/>
+        <v>0.5457349852476208</v>
+      </c>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>['knn', 'svr', 'lightgbm', 'mlp', 'elasticnet']</t>
+        </is>
+      </c>
       <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
+      <c r="AB5" t="n">
+        <v>17.27237718668435</v>
+      </c>
       <c r="AC5" t="n">
-        <v>15.489817892194</v>
+        <v>0.1145294094670146</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.1028335948847694</v>
+        <v>15.32128415191192</v>
       </c>
       <c r="AE5" t="n">
-        <v>13.75166666666667</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>-0.1627501302393579</v>
-      </c>
-      <c r="AG5" t="b">
+        <v>-0.4457659746746545</v>
+      </c>
+      <c r="AF5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>lightgbm</t>
+          <t>svr</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>lightgbm</t>
+          <t>svr</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1015,7 +1010,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{'max_depth': 2}</t>
+          <t>{'kernel': 'linear', 'C': 0.5, 'epsilon': 0.5}</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1039,19 +1034,19 @@
         <v>12</v>
       </c>
       <c r="K6" t="n">
-        <v>15.22148651521338</v>
+        <v>13.60846008092451</v>
       </c>
       <c r="L6" t="n">
-        <v>1.723187129664496</v>
+        <v>2.93345215738552</v>
       </c>
       <c r="M6" t="n">
-        <v>11.94831758892278</v>
+        <v>10.71703143211053</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.05450737862255806</v>
+        <v>0.1571438583372174</v>
       </c>
       <c r="O6" t="n">
-        <v>-1.083223992909056</v>
+        <v>5.771729314177447</v>
       </c>
       <c r="P6" t="n">
         <v>8.600000000000023</v>
@@ -1060,17 +1055,17 @@
         <v>0.95</v>
       </c>
       <c r="R6" t="n">
-        <v>16.00534459691834</v>
+        <v>28.98932912570056</v>
       </c>
       <c r="S6" t="n">
-        <v>9.306629757769668</v>
+        <v>13.15323089766986</v>
       </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="n">
-        <v>7.268316356519059</v>
+        <v>10.04394492268175</v>
       </c>
       <c r="V6" t="n">
-        <v>0.6995841379330299</v>
+        <v>0.3999286750336646</v>
       </c>
       <c r="W6" t="n">
         <v>6</v>
@@ -1081,36 +1076,35 @@
         </is>
       </c>
       <c r="Y6" t="n">
-        <v>17.82620865275871</v>
+        <v>16.18146494284844</v>
       </c>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
+      <c r="AB6" t="n">
+        <v>18.60571260160168</v>
+      </c>
       <c r="AC6" t="n">
-        <v>21.61835417039484</v>
+        <v>0.1254664110610358</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.141928615640495</v>
+        <v>16.6183361615887</v>
       </c>
       <c r="AE6" t="n">
-        <v>19.0132639817008</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>-1.264847829723462</v>
-      </c>
-      <c r="AG6" t="b">
+        <v>-0.6775921658343986</v>
+      </c>
+      <c r="AF6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>mlp</t>
+          <t>lightgbm</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>mlp</t>
+          <t>lightgbm</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1120,12 +1114,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>{'activation': 'tanh', 'hidden_layer_sizes': (25,), 'solver': 'adam', 'random_state': 20}</t>
+          <t>{'max_depth': 2}</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>scale</t>
+          <t>minmax</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -1144,19 +1138,19 @@
         <v>12</v>
       </c>
       <c r="K7" t="n">
-        <v>14.29669440533763</v>
+        <v>15.22148651521338</v>
       </c>
       <c r="L7" t="n">
-        <v>3.993403148375822</v>
+        <v>1.723187129664496</v>
       </c>
       <c r="M7" t="n">
-        <v>10.62350907744359</v>
+        <v>11.94831758892278</v>
       </c>
       <c r="N7" t="n">
-        <v>0.06973483895748134</v>
+        <v>-0.05450737862255806</v>
       </c>
       <c r="O7" t="n">
-        <v>9.941166876312057</v>
+        <v>-1.083223992909056</v>
       </c>
       <c r="P7" t="n">
         <v>8.600000000000023</v>
@@ -1165,17 +1159,17 @@
         <v>0.95</v>
       </c>
       <c r="R7" t="n">
-        <v>22.95450335371923</v>
+        <v>20.47154782925646</v>
       </c>
       <c r="S7" t="n">
-        <v>11.89690823276615</v>
+        <v>9.306629757769668</v>
       </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="n">
-        <v>9.110620603300209</v>
+        <v>7.268316356519059</v>
       </c>
       <c r="V7" t="n">
-        <v>0.5090851049672716</v>
+        <v>0.6995841379330299</v>
       </c>
       <c r="W7" t="n">
         <v>6</v>
@@ -1186,47 +1180,54 @@
         </is>
       </c>
       <c r="Y7" t="n">
-        <v>11.00172937658289</v>
+        <v>19.56241619850066</v>
       </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
+      <c r="AB7" t="n">
+        <v>21.61835417039484</v>
+      </c>
       <c r="AC7" t="n">
-        <v>21.68075545551926</v>
+        <v>0.141928615640495</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.153652488704234</v>
+        <v>19.0132639817008</v>
       </c>
       <c r="AE7" t="n">
-        <v>18.76398861096449</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>-1.277941646897613</v>
-      </c>
-      <c r="AG7" t="b">
+        <v>-1.264847829723462</v>
+      </c>
+      <c r="AF7" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>silverkite</t>
+          <t>mlp</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>silverkite</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['AR1', 'AR2', 'AR3', 'AR4', 'AR12', 'AR24', 'monthsin', 'monthcos', 'year', 'COVID19', 't', 't_COVID19']</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>{'changepoints': 0}</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>{'activation': 'tanh', 'hidden_layer_sizes': (25,), 'solver': 'adam', 'random_state': 20}</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>minmax</t>
+        </is>
+      </c>
       <c r="F8" t="n">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -1235,46 +1236,44 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
         <v>12</v>
       </c>
       <c r="K8" t="n">
-        <v>26.55562683748546</v>
+        <v>13.66207688508325</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1696648171065561</v>
+        <v>2.795035363479342</v>
       </c>
       <c r="M8" t="n">
-        <v>23.02807311996528</v>
+        <v>10.72260302106998</v>
       </c>
       <c r="N8" t="n">
-        <v>-2.417487127820877</v>
+        <v>0.1504891335112754</v>
       </c>
       <c r="O8" t="n">
-        <v>106.261037790605</v>
+        <v>7.549502650113675</v>
       </c>
       <c r="P8" t="n">
-        <v>154.3</v>
+        <v>8.600000000000023</v>
       </c>
       <c r="Q8" t="n">
         <v>0.95</v>
       </c>
       <c r="R8" t="n">
-        <v>72.97749527671445</v>
+        <v>26.21628277079186</v>
       </c>
       <c r="S8" t="n">
-        <v>36.78472798258684</v>
-      </c>
-      <c r="T8" t="n">
-        <v>0.3050851029708435</v>
-      </c>
+        <v>12.67971800182986</v>
+      </c>
+      <c r="T8" t="inlineStr"/>
       <c r="U8" t="n">
-        <v>29.51787617803975</v>
+        <v>9.792161637575065</v>
       </c>
       <c r="V8" t="n">
-        <v>0.06575293074360633</v>
+        <v>0.4423558174861754</v>
       </c>
       <c r="W8" t="n">
         <v>6</v>
@@ -1285,44 +1284,41 @@
         </is>
       </c>
       <c r="Y8" t="n">
-        <v>11.69313794128677</v>
-      </c>
-      <c r="Z8" t="b">
-        <v>1</v>
-      </c>
+        <v>15.70237848470783</v>
+      </c>
+      <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
+      <c r="AB8" t="n">
+        <v>22.89789138252425</v>
+      </c>
       <c r="AC8" t="n">
-        <v>26.55562683748546</v>
+        <v>0.1595180418588098</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.1696648171065561</v>
+        <v>20.80235349703296</v>
       </c>
       <c r="AE8" t="n">
-        <v>23.02807311996528</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>-2.417487127820877</v>
-      </c>
-      <c r="AG8" t="b">
+        <v>-1.540883510360808</v>
+      </c>
+      <c r="AF8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>weighted_level</t>
+          <t>silverkite</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>combo</t>
+          <t>silverkite</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>{'how': 'weighted', 'models': ('arima', 'hwes', 'prophet', 'silverkite'), 'determine_best_by': 'ValidationMetricValue'}</t>
+          <t>{'changepoints': 0}</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -1330,9 +1326,11 @@
         <v>750</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
@@ -1340,19 +1338,19 @@
         <v>12</v>
       </c>
       <c r="K9" t="n">
-        <v>27.7262835200792</v>
+        <v>26.55562683748546</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1962087223154728</v>
+        <v>0.1696648171065561</v>
       </c>
       <c r="M9" t="n">
-        <v>25.93659781662909</v>
+        <v>23.02807311996528</v>
       </c>
       <c r="N9" t="n">
-        <v>-2.725435877421456</v>
+        <v>-2.417487127820877</v>
       </c>
       <c r="O9" t="n">
-        <v>111.2563557055251</v>
+        <v>106.261037790605</v>
       </c>
       <c r="P9" t="n">
         <v>154.3</v>
@@ -1361,65 +1359,64 @@
         <v>0.95</v>
       </c>
       <c r="R9" t="n">
-        <v>37.87482571994885</v>
+        <v>60.36434546891068</v>
       </c>
       <c r="S9" t="n">
-        <v>16.77626852694344</v>
+        <v>36.78472798258684</v>
       </c>
       <c r="T9" t="n">
-        <v>0.1346038924009481</v>
+        <v>0.3050851029708435</v>
       </c>
       <c r="U9" t="n">
-        <v>13.38420218332479</v>
+        <v>29.51787617803975</v>
       </c>
       <c r="V9" t="n">
-        <v>0.8056800525238272</v>
-      </c>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
+        <v>0.06575293074360633</v>
+      </c>
+      <c r="W9" t="n">
+        <v>6</v>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="Y9" t="n">
+        <v>11.69313794128677</v>
+      </c>
       <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>['arima', 'silverkite', 'hwes', 'prophet']</t>
-        </is>
-      </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>(0.4110579036287164, 0.37095419497826587, 0.18061900106313436, 0.03736890032988331)</t>
-        </is>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="n">
+        <v>26.55562683748546</v>
       </c>
       <c r="AC9" t="n">
-        <v>27.7262835200792</v>
+        <v>0.1696648171065561</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.1962087223154728</v>
+        <v>23.02807311996528</v>
       </c>
       <c r="AE9" t="n">
-        <v>25.93659781662909</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>-2.725435877421456</v>
-      </c>
-      <c r="AG9" t="b">
+        <v>-2.417487127820877</v>
+      </c>
+      <c r="AF9" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>hwes</t>
+          <t>weighted_level</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>hwes</t>
+          <t>combo</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>{'trend': 'mul', 'seasonal': 'add'}</t>
+          <t>{'how': 'weighted', 'models': ('arima', 'hwes', 'prophet', 'silverkite'), 'determine_best_by': 'ValidationMetricValue'}</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -1427,11 +1424,9 @@
         <v>750</v>
       </c>
       <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>0</v>
       </c>
@@ -1439,19 +1434,19 @@
         <v>12</v>
       </c>
       <c r="K10" t="n">
-        <v>28.14474040657532</v>
+        <v>27.39289592800548</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1996607260750517</v>
+        <v>0.1917910920715397</v>
       </c>
       <c r="M10" t="n">
-        <v>26.02760101076159</v>
+        <v>25.43305123483565</v>
       </c>
       <c r="N10" t="n">
-        <v>-2.838736193877804</v>
+        <v>-2.636383411693865</v>
       </c>
       <c r="O10" t="n">
-        <v>116.1506821742056</v>
+        <v>110.9472414181668</v>
       </c>
       <c r="P10" t="n">
         <v>154.3</v>
@@ -1460,67 +1455,64 @@
         <v>0.95</v>
       </c>
       <c r="R10" t="n">
-        <v>20.26714080118317</v>
+        <v>38.18615888244086</v>
       </c>
       <c r="S10" t="n">
-        <v>10.84695838401006</v>
+        <v>18.68034782954734</v>
       </c>
       <c r="T10" t="n">
-        <v>0.07961651267651984</v>
+        <v>0.1510355610956562</v>
       </c>
       <c r="U10" t="n">
-        <v>8.517410377583319</v>
+        <v>14.9035417026493</v>
       </c>
       <c r="V10" t="n">
-        <v>0.9187651104570439</v>
-      </c>
-      <c r="W10" t="n">
-        <v>6</v>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>rmse</t>
-        </is>
-      </c>
-      <c r="Y10" t="n">
-        <v>22.0794303743315</v>
-      </c>
-      <c r="Z10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
+        <v>0.759066847298058</v>
+      </c>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>['silverkite', 'arima', 'hwes', 'prophet']</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>(0.43505142517176804, 0.31600989253434564, 0.2093885527328165, 0.03955012956106982)</t>
+        </is>
+      </c>
+      <c r="AB10" t="n">
+        <v>27.39289592800548</v>
+      </c>
       <c r="AC10" t="n">
-        <v>28.14474040657532</v>
+        <v>0.1917910920715397</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.1996607260750517</v>
+        <v>25.43305123483565</v>
       </c>
       <c r="AE10" t="n">
-        <v>26.02760101076159</v>
-      </c>
-      <c r="AF10" t="n">
-        <v>-2.838736193877804</v>
-      </c>
-      <c r="AG10" t="b">
+        <v>-2.636383411693865</v>
+      </c>
+      <c r="AF10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>avg_level</t>
+          <t>hwes</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>combo</t>
+          <t>hwes</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>{'how': 'simple', 'models': ('arima', 'hwes', 'prophet', 'silverkite'), 'determine_best_by': 'ValidationMetricValue'}</t>
+          <t>{'trend': 'mul', 'seasonal': 'add'}</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -1528,9 +1520,11 @@
         <v>750</v>
       </c>
       <c r="G11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
@@ -1538,19 +1532,19 @@
         <v>12</v>
       </c>
       <c r="K11" t="n">
-        <v>27.90285812765169</v>
+        <v>28.14474040657532</v>
       </c>
       <c r="L11" t="n">
-        <v>0.2036016835416031</v>
+        <v>0.1996607260750517</v>
       </c>
       <c r="M11" t="n">
-        <v>26.55895510412931</v>
+        <v>26.02760101076159</v>
       </c>
       <c r="N11" t="n">
-        <v>-2.773037787708755</v>
+        <v>-2.838736193877804</v>
       </c>
       <c r="O11" t="n">
-        <v>113.8014850399619</v>
+        <v>116.1506821742056</v>
       </c>
       <c r="P11" t="n">
         <v>154.3</v>
@@ -1559,148 +1553,138 @@
         <v>0.95</v>
       </c>
       <c r="R11" t="n">
-        <v>34.44808156308144</v>
+        <v>19.51691436914808</v>
       </c>
       <c r="S11" t="n">
-        <v>18.14236106252149</v>
+        <v>10.84695838401006</v>
       </c>
       <c r="T11" t="n">
-        <v>0.1449634070120188</v>
+        <v>0.07961651267651984</v>
       </c>
       <c r="U11" t="n">
-        <v>14.40787998503509</v>
+        <v>8.517410377583319</v>
       </c>
       <c r="V11" t="n">
-        <v>0.7727445756575324</v>
-      </c>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
+        <v>0.9187651104570439</v>
+      </c>
+      <c r="W11" t="n">
+        <v>6</v>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="Y11" t="n">
+        <v>22.0794303743315</v>
+      </c>
       <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>['arima', 'hwes', 'prophet', 'silverkite']</t>
-        </is>
-      </c>
-      <c r="AB11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="n">
+        <v>28.14474040657532</v>
+      </c>
       <c r="AC11" t="n">
-        <v>27.90285812765169</v>
+        <v>0.1996607260750517</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.2036016835416031</v>
+        <v>26.02760101076159</v>
       </c>
       <c r="AE11" t="n">
-        <v>26.55895510412931</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>-2.773037787708755</v>
-      </c>
-      <c r="AG11" t="b">
+        <v>-2.838736193877804</v>
+      </c>
+      <c r="AF11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>svr</t>
+          <t>avg_level</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>svr</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>['AR1', 'AR2', 'AR3', 'AR4', 'AR12', 'AR24', 'monthsin', 'monthcos', 'year', 'COVID19', 't', 't_COVID19']</t>
-        </is>
-      </c>
+          <t>combo</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>{'kernel': 'linear', 'C': 3.0, 'epsilon': 0.5}</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>minmax</t>
-        </is>
-      </c>
+          <t>{'how': 'simple', 'models': ('arima', 'hwes', 'prophet', 'silverkite'), 'determine_best_by': 'ValidationMetricValue'}</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
         <v>12</v>
       </c>
       <c r="K12" t="n">
-        <v>13.95708116936252</v>
+        <v>27.90285812765169</v>
       </c>
       <c r="L12" t="n">
-        <v>3.270854191716512</v>
+        <v>0.2036016835416031</v>
       </c>
       <c r="M12" t="n">
-        <v>10.75923501724551</v>
+        <v>26.55895510412931</v>
       </c>
       <c r="N12" t="n">
-        <v>0.1134061859561084</v>
+        <v>-2.773037787708755</v>
       </c>
       <c r="O12" t="n">
-        <v>9.346164642168484</v>
+        <v>113.8014850399619</v>
       </c>
       <c r="P12" t="n">
-        <v>8.600000000000023</v>
+        <v>154.3</v>
       </c>
       <c r="Q12" t="n">
         <v>0.95</v>
       </c>
       <c r="R12" t="n">
-        <v>19.92324047140101</v>
+        <v>33.30917351513877</v>
       </c>
       <c r="S12" t="n">
-        <v>11.79355779482858</v>
-      </c>
-      <c r="T12" t="inlineStr"/>
+        <v>18.14236106252149</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.1449634070120188</v>
+      </c>
       <c r="U12" t="n">
-        <v>9.103014619399714</v>
+        <v>14.40787998503509</v>
       </c>
       <c r="V12" t="n">
-        <v>0.5175773772721196</v>
-      </c>
-      <c r="W12" t="n">
-        <v>6</v>
-      </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>rmse</t>
-        </is>
-      </c>
-      <c r="Y12" t="n">
-        <v>12.8524516427542</v>
-      </c>
-      <c r="Z12" t="inlineStr"/>
+        <v>0.7727445756575324</v>
+      </c>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>['arima', 'hwes', 'prophet', 'silverkite']</t>
+        </is>
+      </c>
       <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
+      <c r="AB12" t="n">
+        <v>27.90285812765169</v>
+      </c>
       <c r="AC12" t="n">
-        <v>31.07994432706104</v>
+        <v>0.2036016835416031</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.2178783952069605</v>
+        <v>26.55895510412931</v>
       </c>
       <c r="AE12" t="n">
-        <v>28.40806824245395</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>-3.681168104675518</v>
-      </c>
-      <c r="AG12" t="b">
+        <v>-2.773037787708755</v>
+      </c>
+      <c r="AF12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1759,7 +1743,7 @@
         <v>0.95</v>
       </c>
       <c r="R13" t="n">
-        <v>24.35331499490958</v>
+        <v>26.73278856436778</v>
       </c>
       <c r="S13" t="n">
         <v>11.57819485845991</v>
@@ -1782,26 +1766,23 @@
         </is>
       </c>
       <c r="Y13" t="n">
-        <v>9.504741580501653</v>
-      </c>
-      <c r="Z13" t="b">
-        <v>1</v>
-      </c>
+        <v>17.17210821356579</v>
+      </c>
+      <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
+      <c r="AB13" t="n">
+        <v>30.03253838289587</v>
+      </c>
       <c r="AC13" t="n">
-        <v>30.03253838289587</v>
+        <v>0.2218828627261659</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.2218828627261659</v>
+        <v>28.8882370078379</v>
       </c>
       <c r="AE13" t="n">
-        <v>28.8882370078379</v>
-      </c>
-      <c r="AF13" t="n">
         <v>-3.370970289531728</v>
       </c>
-      <c r="AG13" t="b">
+      <c r="AF13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1816,7 +1797,11 @@
           <t>prophet</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>{'n_changepoints': 0}</t>
@@ -1860,7 +1845,7 @@
         <v>0.95</v>
       </c>
       <c r="R14" t="n">
-        <v>59.03651020702416</v>
+        <v>53.59617708675965</v>
       </c>
       <c r="S14" t="n">
         <v>31.51240778559105</v>
@@ -1885,24 +1870,21 @@
       <c r="Y14" t="n">
         <v>29.89636326348532</v>
       </c>
-      <c r="Z14" t="b">
-        <v>1</v>
-      </c>
+      <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
+      <c r="AB14" t="n">
+        <v>30.82740445360642</v>
+      </c>
       <c r="AC14" t="n">
-        <v>30.82740445360642</v>
+        <v>0.2302101922377014</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.2302101922377014</v>
+        <v>29.00782059021475</v>
       </c>
       <c r="AE14" t="n">
-        <v>29.00782059021475</v>
-      </c>
-      <c r="AF14" t="n">
         <v>-3.605403574072794</v>
       </c>
-      <c r="AG14" t="b">
+      <c r="AF14" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1933,57 +1915,57 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>knn</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>elasticnet</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>weighted_diff</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>elasticnet</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>avg_diff</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>knn</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>svr</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>lightgbm</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>mlp</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>silverkite</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>weighted_level</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>hwes</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>avg_level</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>svr</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
@@ -2002,37 +1984,37 @@
         <v>44378</v>
       </c>
       <c r="B2" t="n">
-        <v>156.4644571570697</v>
+        <v>156.2333333333333</v>
       </c>
       <c r="C2" t="n">
-        <v>158.7992090473758</v>
+        <v>154.4829349254608</v>
       </c>
       <c r="D2" t="n">
-        <v>154.3947709099757</v>
+        <v>155.1774371591662</v>
       </c>
       <c r="E2" t="n">
-        <v>152.14</v>
+        <v>154.2018600299367</v>
       </c>
       <c r="F2" t="n">
+        <v>155.7827436835106</v>
+      </c>
+      <c r="G2" t="n">
         <v>148.7214527813213</v>
       </c>
-      <c r="G2" t="n">
-        <v>155.8802695345476</v>
-      </c>
       <c r="H2" t="n">
+        <v>155.7888354260576</v>
+      </c>
+      <c r="I2" t="n">
         <v>106.6355380940402</v>
       </c>
-      <c r="I2" t="n">
-        <v>135.5767138045662</v>
-      </c>
       <c r="J2" t="n">
+        <v>132.536556355982</v>
+      </c>
+      <c r="K2" t="n">
         <v>157.0476009253155</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>133.3205900335453</v>
-      </c>
-      <c r="L2" t="n">
-        <v>156.4329231866341</v>
       </c>
       <c r="M2" t="n">
         <v>154.0837591825671</v>
@@ -2046,37 +2028,37 @@
         <v>44409</v>
       </c>
       <c r="B3" t="n">
-        <v>153.2199405143319</v>
+        <v>151.9</v>
       </c>
       <c r="C3" t="n">
-        <v>154.4029773424122</v>
+        <v>154.2126089521852</v>
       </c>
       <c r="D3" t="n">
-        <v>151.509338527181</v>
+        <v>152.7254024022442</v>
       </c>
       <c r="E3" t="n">
-        <v>149.335</v>
+        <v>151.5180484200912</v>
       </c>
       <c r="F3" t="n">
+        <v>152.2880811434019</v>
+      </c>
+      <c r="G3" t="n">
         <v>146.9128640726533</v>
       </c>
-      <c r="G3" t="n">
-        <v>153.6669665590815</v>
-      </c>
       <c r="H3" t="n">
+        <v>152.2766879322158</v>
+      </c>
+      <c r="I3" t="n">
         <v>106.5853620249925</v>
       </c>
-      <c r="I3" t="n">
-        <v>132.3520832182172</v>
-      </c>
       <c r="J3" t="n">
+        <v>129.6590184256368</v>
+      </c>
+      <c r="K3" t="n">
         <v>151.793511285846</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>130.1929599155089</v>
-      </c>
-      <c r="L3" t="n">
-        <v>153.2288846617579</v>
       </c>
       <c r="M3" t="n">
         <v>148.7645249869927</v>
@@ -2090,37 +2072,37 @@
         <v>44440</v>
       </c>
       <c r="B4" t="n">
-        <v>149.834595332619</v>
+        <v>153.0555555555556</v>
       </c>
       <c r="C4" t="n">
-        <v>152.7763478640812</v>
+        <v>153.6581618432003</v>
       </c>
       <c r="D4" t="n">
-        <v>148.3707073040165</v>
+        <v>149.5310689364056</v>
       </c>
       <c r="E4" t="n">
-        <v>147.385</v>
+        <v>148.5395261073733</v>
       </c>
       <c r="F4" t="n">
+        <v>146.2916067907757</v>
+      </c>
+      <c r="G4" t="n">
         <v>144.8067994001438</v>
       </c>
-      <c r="G4" t="n">
-        <v>149.5862896993246</v>
-      </c>
       <c r="H4" t="n">
+        <v>144.8855069471908</v>
+      </c>
+      <c r="I4" t="n">
         <v>106.553965064259</v>
       </c>
-      <c r="I4" t="n">
-        <v>131.946612394645</v>
-      </c>
       <c r="J4" t="n">
+        <v>129.304319678604</v>
+      </c>
+      <c r="K4" t="n">
         <v>152.2990677021062</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>128.4636836774558</v>
-      </c>
-      <c r="L4" t="n">
-        <v>147.2990995565332</v>
       </c>
       <c r="M4" t="n">
         <v>148.2054139097186</v>
@@ -2134,37 +2116,37 @@
         <v>44470</v>
       </c>
       <c r="B5" t="n">
-        <v>147.9501042937287</v>
+        <v>152.5</v>
       </c>
       <c r="C5" t="n">
-        <v>154.2175198679189</v>
+        <v>153.0670682989847</v>
       </c>
       <c r="D5" t="n">
-        <v>146.7962079348846</v>
+        <v>146.0904011132333</v>
       </c>
       <c r="E5" t="n">
-        <v>146.015</v>
+        <v>145.7707250940874</v>
       </c>
       <c r="F5" t="n">
+        <v>140.3745447770864</v>
+      </c>
+      <c r="G5" t="n">
         <v>145.740975140968</v>
       </c>
-      <c r="G5" t="n">
-        <v>145.7565794100106</v>
-      </c>
       <c r="H5" t="n">
+        <v>137.1710372533977</v>
+      </c>
+      <c r="I5" t="n">
         <v>106.5178894708137</v>
       </c>
-      <c r="I5" t="n">
-        <v>132.4770738233643</v>
-      </c>
       <c r="J5" t="n">
+        <v>129.8213248513322</v>
+      </c>
+      <c r="K5" t="n">
         <v>153.1684556923884</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>130.0263471812167</v>
-      </c>
-      <c r="L5" t="n">
-        <v>142.2509652555254</v>
       </c>
       <c r="M5" t="n">
         <v>148.6988074281037</v>
@@ -2178,37 +2160,37 @@
         <v>44501</v>
       </c>
       <c r="B6" t="n">
-        <v>137.5012238417074</v>
+        <v>142.3777777777778</v>
       </c>
       <c r="C6" t="n">
-        <v>144.1350916144025</v>
+        <v>152.3912689279172</v>
       </c>
       <c r="D6" t="n">
-        <v>136.8354830699202</v>
+        <v>139.5225438304855</v>
       </c>
       <c r="E6" t="n">
-        <v>139.04</v>
+        <v>137.7927528499069</v>
       </c>
       <c r="F6" t="n">
+        <v>131.9098722817563</v>
+      </c>
+      <c r="G6" t="n">
         <v>135.6621590991136</v>
       </c>
-      <c r="G6" t="n">
-        <v>134.6056226616592</v>
-      </c>
       <c r="H6" t="n">
+        <v>126.6226861629697</v>
+      </c>
+      <c r="I6" t="n">
         <v>106.4781132810161</v>
       </c>
-      <c r="I6" t="n">
-        <v>123.8608529697058</v>
-      </c>
       <c r="J6" t="n">
+        <v>122.0013415938842</v>
+      </c>
+      <c r="K6" t="n">
         <v>139.6313984936843</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>117.9464977327946</v>
-      </c>
-      <c r="L6" t="n">
-        <v>130.7345419744258</v>
       </c>
       <c r="M6" t="n">
         <v>135.6983592177467</v>
@@ -2222,37 +2204,37 @@
         <v>44531</v>
       </c>
       <c r="B7" t="n">
-        <v>135.5841283572167</v>
+        <v>134.8444444444445</v>
       </c>
       <c r="C7" t="n">
-        <v>145.4080760158442</v>
+        <v>152.1247543370455</v>
       </c>
       <c r="D7" t="n">
-        <v>133.8725988432035</v>
+        <v>136.1555441254717</v>
       </c>
       <c r="E7" t="n">
-        <v>135.38</v>
+        <v>133.486197810462</v>
       </c>
       <c r="F7" t="n">
+        <v>128.6019709344622</v>
+      </c>
+      <c r="G7" t="n">
         <v>130.1284097245064</v>
       </c>
-      <c r="G7" t="n">
-        <v>130.609724761436</v>
-      </c>
       <c r="H7" t="n">
+        <v>121.7314096118514</v>
+      </c>
+      <c r="I7" t="n">
         <v>106.4538423695216</v>
       </c>
-      <c r="I7" t="n">
-        <v>118.6068900136348</v>
-      </c>
       <c r="J7" t="n">
+        <v>117.1230215705475</v>
+      </c>
+      <c r="K7" t="n">
         <v>130.1452750396012</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>109.9245552130608</v>
-      </c>
-      <c r="L7" t="n">
-        <v>127.8367837142309</v>
       </c>
       <c r="M7" t="n">
         <v>128.5054964604076</v>
@@ -2266,37 +2248,37 @@
         <v>44562</v>
       </c>
       <c r="B8" t="n">
-        <v>135.1977095916556</v>
+        <v>136.0333333333334</v>
       </c>
       <c r="C8" t="n">
-        <v>146.3485760593025</v>
+        <v>152.2302680683478</v>
       </c>
       <c r="D8" t="n">
-        <v>133.3118424825736</v>
+        <v>136.3156120314064</v>
       </c>
       <c r="E8" t="n">
-        <v>134.525</v>
+        <v>133.5537898903738</v>
       </c>
       <c r="F8" t="n">
+        <v>128.6521872686355</v>
+      </c>
+      <c r="G8" t="n">
         <v>129.319792539172</v>
       </c>
-      <c r="G8" t="n">
-        <v>128.6765892753957</v>
-      </c>
       <c r="H8" t="n">
+        <v>121.5333682423802</v>
+      </c>
+      <c r="I8" t="n">
         <v>106.369725374985</v>
       </c>
-      <c r="I8" t="n">
-        <v>118.4215222781078</v>
-      </c>
       <c r="J8" t="n">
+        <v>116.6970307362043</v>
+      </c>
+      <c r="K8" t="n">
         <v>127.0347945577791</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>108.292595138963</v>
-      </c>
-      <c r="L8" t="n">
-        <v>127.6892545389978</v>
       </c>
       <c r="M8" t="n">
         <v>129.9296949461466</v>
@@ -2310,37 +2292,37 @@
         <v>44593</v>
       </c>
       <c r="B9" t="n">
-        <v>131.8493663493862</v>
+        <v>135.7888888888889</v>
       </c>
       <c r="C9" t="n">
-        <v>140.1731985490464</v>
+        <v>152.5843713444252</v>
       </c>
       <c r="D9" t="n">
-        <v>131.8881850509773</v>
+        <v>137.1824831635823</v>
       </c>
       <c r="E9" t="n">
-        <v>136.91</v>
+        <v>134.5532647353921</v>
       </c>
       <c r="F9" t="n">
+        <v>129.9371495826001</v>
+      </c>
+      <c r="G9" t="n">
         <v>131.1034662548581</v>
       </c>
-      <c r="G9" t="n">
-        <v>124.6562138372123</v>
-      </c>
       <c r="H9" t="n">
+        <v>123.3524476061881</v>
+      </c>
+      <c r="I9" t="n">
         <v>106.3954678735738</v>
       </c>
-      <c r="I9" t="n">
-        <v>116.906247364058</v>
-      </c>
       <c r="J9" t="n">
+        <v>115.1585625410479</v>
+      </c>
+      <c r="K9" t="n">
         <v>121.4133577577672</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>106.9844172987016</v>
-      </c>
-      <c r="L9" t="n">
-        <v>126.5980466137695</v>
       </c>
       <c r="M9" t="n">
         <v>128.5300011600411</v>
@@ -2354,37 +2336,37 @@
         <v>44621</v>
       </c>
       <c r="B10" t="n">
-        <v>145.9665870493995</v>
+        <v>147.6111111111111</v>
       </c>
       <c r="C10" t="n">
-        <v>155.3282959238043</v>
+        <v>153.4976076391647</v>
       </c>
       <c r="D10" t="n">
-        <v>145.5251354552358</v>
+        <v>144.5956615919819</v>
       </c>
       <c r="E10" t="n">
-        <v>147.385</v>
+        <v>144.1378677822435</v>
       </c>
       <c r="F10" t="n">
+        <v>138.9310644740486</v>
+      </c>
+      <c r="G10" t="n">
         <v>145.7901504982587</v>
       </c>
-      <c r="G10" t="n">
-        <v>139.1754065000975</v>
-      </c>
       <c r="H10" t="n">
+        <v>134.8594051886341</v>
+      </c>
+      <c r="I10" t="n">
         <v>106.3690582836884</v>
       </c>
-      <c r="I10" t="n">
-        <v>127.1327946370347</v>
-      </c>
       <c r="J10" t="n">
+        <v>124.352485963539</v>
+      </c>
+      <c r="K10" t="n">
         <v>135.9388755949252</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>121.7801238125869</v>
-      </c>
-      <c r="L10" t="n">
-        <v>139.9468243540186</v>
       </c>
       <c r="M10" t="n">
         <v>144.4335414030003</v>
@@ -2398,37 +2380,37 @@
         <v>44652</v>
       </c>
       <c r="B11" t="n">
-        <v>142.6034371372044</v>
+        <v>155.6888888888889</v>
       </c>
       <c r="C11" t="n">
-        <v>145.517811401481</v>
+        <v>154.188179796974</v>
       </c>
       <c r="D11" t="n">
-        <v>144.8022237615411</v>
+        <v>148.2940720812412</v>
       </c>
       <c r="E11" t="n">
-        <v>154.95</v>
+        <v>147.8843003227836</v>
       </c>
       <c r="F11" t="n">
+        <v>142.7525479761617</v>
+      </c>
+      <c r="G11" t="n">
         <v>146.4682608757153</v>
       </c>
-      <c r="G11" t="n">
-        <v>136.9738526779404</v>
-      </c>
       <c r="H11" t="n">
+        <v>140.3236240761777</v>
+      </c>
+      <c r="I11" t="n">
         <v>106.3350629169357</v>
       </c>
-      <c r="I11" t="n">
-        <v>131.0869694669516</v>
-      </c>
       <c r="J11" t="n">
+        <v>128.0321429096545</v>
+      </c>
+      <c r="K11" t="n">
         <v>142.7182220353752</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>128.6355934304664</v>
-      </c>
-      <c r="L11" t="n">
-        <v>140.1011938525688</v>
       </c>
       <c r="M11" t="n">
         <v>149.7043619596769</v>
@@ -2442,37 +2424,37 @@
         <v>44682</v>
       </c>
       <c r="B12" t="n">
-        <v>152.4993404939964</v>
+        <v>155.9222222222222</v>
       </c>
       <c r="C12" t="n">
-        <v>154.4316603895961</v>
+        <v>155.0651516864054</v>
       </c>
       <c r="D12" t="n">
-        <v>152.8580976897081</v>
+        <v>152.9890438922299</v>
       </c>
       <c r="E12" t="n">
-        <v>158.165</v>
+        <v>152.5752937766709</v>
       </c>
       <c r="F12" t="n">
+        <v>150.9067314288149</v>
+      </c>
+      <c r="G12" t="n">
         <v>150.6788229802307</v>
       </c>
-      <c r="G12" t="n">
-        <v>149.4102194785826</v>
-      </c>
       <c r="H12" t="n">
+        <v>150.3035405656811</v>
+      </c>
+      <c r="I12" t="n">
         <v>106.2989957631332</v>
       </c>
-      <c r="I12" t="n">
-        <v>134.839492824787</v>
-      </c>
       <c r="J12" t="n">
+        <v>131.6173576921419</v>
+      </c>
+      <c r="K12" t="n">
         <v>151.7653119580748</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>133.6058301880265</v>
-      </c>
-      <c r="L12" t="n">
-        <v>151.6047856001314</v>
       </c>
       <c r="M12" t="n">
         <v>154.3221835811966</v>
@@ -2486,37 +2468,37 @@
         <v>44713</v>
       </c>
       <c r="B13" t="n">
-        <v>161.6227270113856</v>
+        <v>156.0888888888889</v>
       </c>
       <c r="C13" t="n">
-        <v>165.0735337264939</v>
+        <v>155.7600702125228</v>
       </c>
       <c r="D13" t="n">
-        <v>159.4139783079057</v>
+        <v>156.8853534314543</v>
       </c>
       <c r="E13" t="n">
-        <v>160.39</v>
+        <v>155.8699037515689</v>
       </c>
       <c r="F13" t="n">
+        <v>157.9429787561425</v>
+      </c>
+      <c r="G13" t="n">
         <v>150.6968212911885</v>
       </c>
-      <c r="G13" t="n">
-        <v>158.5976133084345</v>
-      </c>
       <c r="H13" t="n">
+        <v>158.8607596091017</v>
+      </c>
+      <c r="I13" t="n">
         <v>106.261037790605</v>
       </c>
-      <c r="I13" t="n">
-        <v>138.035724974303</v>
-      </c>
       <c r="J13" t="n">
+        <v>134.5916219273634</v>
+      </c>
+      <c r="K13" t="n">
         <v>159.3885013282707</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>136.3040108057341</v>
-      </c>
-      <c r="L13" t="n">
-        <v>162.3119232134116</v>
       </c>
       <c r="M13" t="n">
         <v>158.9077066775396</v>
@@ -2530,37 +2512,37 @@
         <v>44743</v>
       </c>
       <c r="B14" t="n">
-        <v>165.9685495119011</v>
+        <v>157.7888888888889</v>
       </c>
       <c r="C14" t="n">
-        <v>171.7645794638347</v>
+        <v>156.0265099393303</v>
       </c>
       <c r="D14" t="n">
-        <v>162.054753060714</v>
+        <v>158.6030053849536</v>
       </c>
       <c r="E14" t="n">
-        <v>159.22</v>
+        <v>157.3434416914807</v>
       </c>
       <c r="F14" t="n">
+        <v>160.5797369209502</v>
+      </c>
+      <c r="G14" t="n">
         <v>150.1935956517792</v>
       </c>
-      <c r="G14" t="n">
-        <v>162.1714564859708</v>
-      </c>
       <c r="H14" t="n">
+        <v>162.1284770564549</v>
+      </c>
+      <c r="I14" t="n">
         <v>106.2352700661455</v>
       </c>
-      <c r="I14" t="n">
-        <v>139.0598332248966</v>
-      </c>
       <c r="J14" t="n">
+        <v>135.5361758670852</v>
+      </c>
+      <c r="K14" t="n">
         <v>162.4566424611881</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>136.1949251933029</v>
-      </c>
-      <c r="L14" t="n">
-        <v>166.9241337019853</v>
       </c>
       <c r="M14" t="n">
         <v>160.5387370004248</v>
@@ -2574,37 +2556,37 @@
         <v>44774</v>
       </c>
       <c r="B15" t="n">
-        <v>160.6796039292746</v>
+        <v>154.3111111111111</v>
       </c>
       <c r="C15" t="n">
-        <v>165.3232734144235</v>
+        <v>155.7175641069931</v>
       </c>
       <c r="D15" t="n">
-        <v>157.0619914355553</v>
+        <v>155.4082494624846</v>
       </c>
       <c r="E15" t="n">
-        <v>156.5</v>
+        <v>153.4178459603911</v>
       </c>
       <c r="F15" t="n">
+        <v>155.7804621835373</v>
+      </c>
+      <c r="G15" t="n">
         <v>144.5309593385967</v>
       </c>
-      <c r="G15" t="n">
-        <v>158.0529748937293</v>
-      </c>
       <c r="H15" t="n">
+        <v>156.7491330617171</v>
+      </c>
+      <c r="I15" t="n">
         <v>106.1949154309407</v>
       </c>
-      <c r="I15" t="n">
-        <v>135.7453182856275</v>
-      </c>
       <c r="J15" t="n">
+        <v>132.5860567724467</v>
+      </c>
+      <c r="K15" t="n">
         <v>157.2253245670919</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>132.8783197309156</v>
-      </c>
-      <c r="L15" t="n">
-        <v>160.9027495310272</v>
       </c>
       <c r="M15" t="n">
         <v>155.0370636915559</v>
@@ -2618,37 +2600,37 @@
         <v>44805</v>
       </c>
       <c r="B16" t="n">
-        <v>158.1167222938341</v>
+        <v>155.6</v>
       </c>
       <c r="C16" t="n">
-        <v>165.4144051156462</v>
+        <v>155.2436903861643</v>
       </c>
       <c r="D16" t="n">
-        <v>154.2426954082276</v>
+        <v>152.2250158617255</v>
       </c>
       <c r="E16" t="n">
-        <v>156.055</v>
+        <v>150.0804912537835</v>
       </c>
       <c r="F16" t="n">
+        <v>150.079653726873</v>
+      </c>
+      <c r="G16" t="n">
         <v>140.2590080892442</v>
       </c>
-      <c r="G16" t="n">
-        <v>154.395544669755</v>
-      </c>
       <c r="H16" t="n">
+        <v>149.2201040666356</v>
+      </c>
+      <c r="I16" t="n">
         <v>106.1672793326401</v>
       </c>
-      <c r="I16" t="n">
-        <v>135.3184673685595</v>
-      </c>
       <c r="J16" t="n">
+        <v>132.2246753167979</v>
+      </c>
+      <c r="K16" t="n">
         <v>157.7537485964286</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>131.2984648390621</v>
-      </c>
-      <c r="L16" t="n">
-        <v>155.0895191664923</v>
       </c>
       <c r="M16" t="n">
         <v>154.3488471417564</v>
@@ -2662,37 +2644,37 @@
         <v>44835</v>
       </c>
       <c r="B17" t="n">
-        <v>155.1491313002568</v>
+        <v>153.6</v>
       </c>
       <c r="C17" t="n">
-        <v>166.0340388294437</v>
+        <v>154.661033975012</v>
       </c>
       <c r="D17" t="n">
-        <v>152.2752101475293</v>
+        <v>148.1405085479697</v>
       </c>
       <c r="E17" t="n">
-        <v>154.685</v>
+        <v>147.0493297990561</v>
       </c>
       <c r="F17" t="n">
+        <v>143.3556746454981</v>
+      </c>
+      <c r="G17" t="n">
         <v>143.4112579515753</v>
       </c>
-      <c r="G17" t="n">
-        <v>149.1678979755925</v>
-      </c>
       <c r="H17" t="n">
+        <v>140.2186824231951</v>
+      </c>
+      <c r="I17" t="n">
         <v>106.1176214429189</v>
       </c>
-      <c r="I17" t="n">
-        <v>135.803773279416</v>
-      </c>
       <c r="J17" t="n">
+        <v>132.6866240507931</v>
+      </c>
+      <c r="K17" t="n">
         <v>158.6461004710874</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>132.4180797935436</v>
-      </c>
-      <c r="L17" t="n">
-        <v>148.077855981035</v>
       </c>
       <c r="M17" t="n">
         <v>154.9019446006173</v>
@@ -2706,37 +2688,37 @@
         <v>44866</v>
       </c>
       <c r="B18" t="n">
-        <v>145.1239658616179</v>
+        <v>144.1333333333333</v>
       </c>
       <c r="C18" t="n">
-        <v>156.6569818433282</v>
+        <v>154.0511771537961</v>
       </c>
       <c r="D18" t="n">
-        <v>142.7299978743849</v>
+        <v>141.8431810890497</v>
       </c>
       <c r="E18" t="n">
-        <v>147.71</v>
+        <v>139.4854433265807</v>
       </c>
       <c r="F18" t="n">
+        <v>135.24403506868</v>
+      </c>
+      <c r="G18" t="n">
         <v>134.1583843833632</v>
       </c>
-      <c r="G18" t="n">
-        <v>138.3720945258295</v>
-      </c>
       <c r="H18" t="n">
+        <v>129.8402866937306</v>
+      </c>
+      <c r="I18" t="n">
         <v>106.0778452531214</v>
       </c>
-      <c r="I18" t="n">
-        <v>127.2546841897325</v>
-      </c>
       <c r="J18" t="n">
+        <v>124.9388210508214</v>
+      </c>
+      <c r="K18" t="n">
         <v>145.132103833357</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>120.7801494857001</v>
-      </c>
-      <c r="L18" t="n">
-        <v>136.7525286194038</v>
       </c>
       <c r="M18" t="n">
         <v>141.8955347671984</v>
@@ -2750,37 +2732,37 @@
         <v>44896</v>
       </c>
       <c r="B19" t="n">
-        <v>142.1106498325072</v>
+        <v>136.6</v>
       </c>
       <c r="C19" t="n">
-        <v>157.2379678810412</v>
+        <v>153.7559056674021</v>
       </c>
       <c r="D19" t="n">
-        <v>138.8563974260757</v>
+        <v>138.0581859442526</v>
       </c>
       <c r="E19" t="n">
-        <v>143.02</v>
+        <v>134.8221680592271</v>
       </c>
       <c r="F19" t="n">
+        <v>131.1356439006925</v>
+      </c>
+      <c r="G19" t="n">
         <v>128.624635008756</v>
       </c>
-      <c r="G19" t="n">
-        <v>132.7653227960875</v>
-      </c>
       <c r="H19" t="n">
+        <v>123.9946557192847</v>
+      </c>
+      <c r="I19" t="n">
         <v>106.0535743416269</v>
       </c>
-      <c r="I19" t="n">
-        <v>121.9768352490134</v>
-      </c>
       <c r="J19" t="n">
+        <v>120.0361371515036</v>
+      </c>
+      <c r="K19" t="n">
         <v>135.669138023847</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>112.5865950048163</v>
-      </c>
-      <c r="L19" t="n">
-        <v>132.6340614444936</v>
       </c>
       <c r="M19" t="n">
         <v>134.69852011225</v>
@@ -2794,37 +2776,37 @@
         <v>44927</v>
       </c>
       <c r="B20" t="n">
-        <v>140.726761389177</v>
+        <v>137.7888888888889</v>
       </c>
       <c r="C20" t="n">
-        <v>156.9602196007386</v>
+        <v>153.8342323849369</v>
       </c>
       <c r="D20" t="n">
-        <v>137.4398745987818</v>
+        <v>137.9520677097071</v>
       </c>
       <c r="E20" t="n">
-        <v>142.285</v>
+        <v>134.4566713776896</v>
       </c>
       <c r="F20" t="n">
+        <v>130.7351858841903</v>
+      </c>
+      <c r="G20" t="n">
         <v>126.6212647893373</v>
       </c>
-      <c r="G20" t="n">
-        <v>129.5732430346916</v>
-      </c>
       <c r="H20" t="n">
+        <v>123.3037849410947</v>
+      </c>
+      <c r="I20" t="n">
         <v>105.9833694873133</v>
       </c>
-      <c r="I20" t="n">
-        <v>121.7933752840314</v>
-      </c>
       <c r="J20" t="n">
+        <v>119.6129501025123</v>
+      </c>
+      <c r="K20" t="n">
         <v>132.5819126789138</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>110.9092396395944</v>
-      </c>
-      <c r="L20" t="n">
-        <v>131.7596455691414</v>
       </c>
       <c r="M20" t="n">
         <v>136.1246482049059</v>
@@ -2838,37 +2820,37 @@
         <v>44958</v>
       </c>
       <c r="B21" t="n">
-        <v>137.7985441286764</v>
+        <v>138.6888888888889</v>
       </c>
       <c r="C21" t="n">
-        <v>150.1107340855679</v>
+        <v>154.203383688048</v>
       </c>
       <c r="D21" t="n">
-        <v>136.897869755064</v>
+        <v>139.3727024217588</v>
       </c>
       <c r="E21" t="n">
-        <v>146.13</v>
+        <v>136.3280065861924</v>
       </c>
       <c r="F21" t="n">
+        <v>132.4446187478776</v>
+      </c>
+      <c r="G21" t="n">
         <v>130.2945183016463</v>
       </c>
-      <c r="G21" t="n">
-        <v>126.5284530373973</v>
-      </c>
       <c r="H21" t="n">
+        <v>126.0086233045012</v>
+      </c>
+      <c r="I21" t="n">
         <v>105.9994957483446</v>
       </c>
-      <c r="I21" t="n">
-        <v>120.3419523991321</v>
-      </c>
       <c r="J21" t="n">
+        <v>118.1421016713971</v>
+      </c>
+      <c r="K21" t="n">
         <v>126.9838289185437</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>110.0278025248553</v>
-      </c>
-      <c r="L21" t="n">
-        <v>131.4256433507084</v>
       </c>
       <c r="M21" t="n">
         <v>134.7247596385261</v>
@@ -2882,37 +2864,37 @@
         <v>44986</v>
       </c>
       <c r="B22" t="n">
-        <v>154.7646569970727</v>
+        <v>149.3444444444445</v>
       </c>
       <c r="C22" t="n">
-        <v>169.9909621703721</v>
+        <v>155.1503712924139</v>
       </c>
       <c r="D22" t="n">
-        <v>152.6939293880108</v>
+        <v>147.4195971796331</v>
       </c>
       <c r="E22" t="n">
-        <v>154.65</v>
+        <v>146.8859555699502</v>
       </c>
       <c r="F22" t="n">
+        <v>142.9174798006438</v>
+      </c>
+      <c r="G22" t="n">
         <v>147.9095168858211</v>
       </c>
-      <c r="G22" t="n">
-        <v>142.6407895794378</v>
-      </c>
       <c r="H22" t="n">
+        <v>139.1079654264277</v>
+      </c>
+      <c r="I22" t="n">
         <v>105.9687902557937</v>
       </c>
-      <c r="I22" t="n">
-        <v>130.4757501808952</v>
-      </c>
       <c r="J22" t="n">
+        <v>127.2381227978515</v>
+      </c>
+      <c r="K22" t="n">
         <v>141.5327981102608</v>
       </c>
-      <c r="K22" t="n">
+      <c r="L22" t="n">
         <v>124.1904561813305</v>
-      </c>
-      <c r="L22" t="n">
-        <v>148.2783783044231</v>
       </c>
       <c r="M22" t="n">
         <v>150.6281663650286</v>
@@ -2926,37 +2908,37 @@
         <v>45017</v>
       </c>
       <c r="B23" t="n">
-        <v>154.5733749060052</v>
+        <v>159.2777777777778</v>
       </c>
       <c r="C23" t="n">
-        <v>162.5441278968059</v>
+        <v>155.9600200270807</v>
       </c>
       <c r="D23" t="n">
-        <v>154.8531731254361</v>
+        <v>152.892521055846</v>
       </c>
       <c r="E23" t="n">
-        <v>161.845</v>
+        <v>152.9532293977424</v>
       </c>
       <c r="F23" t="n">
+        <v>149.2170833773084</v>
+      </c>
+      <c r="G23" t="n">
         <v>152.5683948711254</v>
       </c>
-      <c r="G23" t="n">
-        <v>145.0016501493731</v>
-      </c>
       <c r="H23" t="n">
+        <v>147.7428709354197</v>
+      </c>
+      <c r="I23" t="n">
         <v>105.9186141867459</v>
       </c>
-      <c r="I23" t="n">
-        <v>134.4417771412856</v>
-      </c>
       <c r="J23" t="n">
+        <v>130.9300587210212</v>
+      </c>
+      <c r="K23" t="n">
         <v>148.3356946340875</v>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>131.1386025868964</v>
-      </c>
-      <c r="L23" t="n">
-        <v>152.3066927098762</v>
       </c>
       <c r="M23" t="n">
         <v>155.8990492848793</v>
@@ -2970,37 +2952,37 @@
         <v>45047</v>
       </c>
       <c r="B24" t="n">
-        <v>164.1658334785363</v>
+        <v>160.7111111111111</v>
       </c>
       <c r="C24" t="n">
-        <v>171.0071566779579</v>
+        <v>156.7805853976646</v>
       </c>
       <c r="D24" t="n">
-        <v>162.8504926241115</v>
+        <v>157.7091708425497</v>
       </c>
       <c r="E24" t="n">
-        <v>164.025</v>
+        <v>158.1082276174045</v>
       </c>
       <c r="F24" t="n">
+        <v>157.0763052910096</v>
+      </c>
+      <c r="G24" t="n">
         <v>158.3870570061465</v>
       </c>
-      <c r="G24" t="n">
-        <v>157.3138949409713</v>
-      </c>
       <c r="H24" t="n">
+        <v>157.5860792810907</v>
+      </c>
+      <c r="I24" t="n">
         <v>105.9091276144887</v>
       </c>
-      <c r="I24" t="n">
-        <v>138.275117461052</v>
-      </c>
       <c r="J24" t="n">
+        <v>134.6023677738834</v>
+      </c>
+      <c r="K24" t="n">
         <v>157.4064337846238</v>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>136.5675409232188</v>
-      </c>
-      <c r="L24" t="n">
-        <v>163.5193544954819</v>
       </c>
       <c r="M24" t="n">
         <v>160.5168645434145</v>
@@ -3014,37 +2996,37 @@
         <v>45078</v>
       </c>
       <c r="B25" t="n">
-        <v>170.2481039075256</v>
+        <v>162.5555555555556</v>
       </c>
       <c r="C25" t="n">
-        <v>177.7519649006346</v>
+        <v>157.3403690609455</v>
       </c>
       <c r="D25" t="n">
-        <v>166.7439919084075</v>
+        <v>160.8402832999173</v>
       </c>
       <c r="E25" t="n">
-        <v>165.805</v>
+        <v>160.3263675065341</v>
       </c>
       <c r="F25" t="n">
+        <v>162.3078993100053</v>
+      </c>
+      <c r="G25" t="n">
         <v>155.2820380120935</v>
       </c>
-      <c r="G25" t="n">
-        <v>163.672599484132</v>
-      </c>
       <c r="H25" t="n">
+        <v>164.1459755940706</v>
+      </c>
+      <c r="I25" t="n">
         <v>105.8679007802696</v>
       </c>
-      <c r="I25" t="n">
-        <v>141.4111153189299</v>
-      </c>
       <c r="J25" t="n">
+        <v>137.5131764612125</v>
+      </c>
+      <c r="K25" t="n">
         <v>165.0533719445087</v>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>138.8472970021653</v>
-      </c>
-      <c r="L25" t="n">
-        <v>171.2083571451774</v>
       </c>
       <c r="M25" t="n">
         <v>165.1023833462817</v>

</xml_diff>